<commit_message>
properly detect time and fixed some audio
</commit_message>
<xml_diff>
--- a/calendar_times.xlsx
+++ b/calendar_times.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiperl\Documents\GitHub\GatorWatch2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -42,34 +37,74 @@
     <t>Time</t>
   </si>
   <si>
+    <t>Coco</t>
+  </si>
+  <si>
+    <t>Royal Park</t>
+  </si>
+  <si>
     <t>Dec 3</t>
   </si>
   <si>
-    <t>Coco</t>
-  </si>
-  <si>
-    <t>Royal Park</t>
-  </si>
-  <si>
     <t>10:10pm</t>
+  </si>
+  <si>
+    <t>Shark Tank</t>
+  </si>
+  <si>
+    <t>Episode 904</t>
+  </si>
+  <si>
+    <t>(Season 9, Episode 2)</t>
+  </si>
+  <si>
+    <t>Rohan Oza sits in with the sharks. Products include ultimate survival kits; a wireless microphone designed to engage kids; and an app to navigate airports.</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>10:00pm</t>
+  </si>
+  <si>
+    <t>Star Trek: Voyager</t>
+  </si>
+  <si>
+    <t>Unimatrix Zero</t>
+  </si>
+  <si>
+    <t>(Season 6, Episode 26)</t>
+  </si>
+  <si>
+    <t>Part 1 of two. Seven of Nine is drawn into a dreamworld that Borg drones inhabit during their sleep cycles---a threat to the Borg Queen's control that Janeway wants to exploit. Borg Queen: Susanna Thompson. Axum: Mark Deakins. Korok: Jerome Butler. Laura: (more…)Part 1 of two. Seven of Nine is drawn into a dreamworld that Borg drones inhabit during their sleep cycles---a threat to the Borg Queen's control that Janeway wants to exploit. Borg Queen: Susanna Thompson. Axum: Mark Deakins. Korok: Jerome Butler. Laura: Joanna Heimbold. Seven of Nine: Jeri Ryan. Janeway: Kate Mulgrew.</t>
+  </si>
+  <si>
+    <t>BBC</t>
+  </si>
+  <si>
+    <t>Dec 4</t>
+  </si>
+  <si>
+    <t>8:00pm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -85,25 +120,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -403,16 +429,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,28 +465,68 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F3" s="1"/>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F4" s="1"/>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed wrong intent issue
</commit_message>
<xml_diff>
--- a/calendar_times.xlsx
+++ b/calendar_times.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -86,6 +86,27 @@
   </si>
   <si>
     <t>8:00pm</t>
+  </si>
+  <si>
+    <t>1:10pm</t>
+  </si>
+  <si>
+    <t>Episode 307</t>
+  </si>
+  <si>
+    <t>(Season 3, Episode 2)</t>
+  </si>
+  <si>
+    <t>Ideas include a training system for salespeople, a management system for cargo trucks, family-friendly Las Vegas entertainment and a cat-portrait business. Also: a follow-up on a Season 2 potty-training product for cats.</t>
+  </si>
+  <si>
+    <t>CNBC</t>
+  </si>
+  <si>
+    <t>Dec 5</t>
+  </si>
+  <si>
+    <t>7:00pm</t>
   </si>
 </sst>
 </file>
@@ -434,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
@@ -525,6 +546,46 @@
         <v>23</v>
       </c>
     </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s"/>
+      <c r="C5" t="s"/>
+      <c r="D5" t="s"/>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>